<commit_message>
Reverted to version 3
</commit_message>
<xml_diff>
--- a/Excel/Excel Test.xlsx
+++ b/Excel/Excel Test.xlsx
@@ -345,19 +345,21 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="90.75" x14ac:dyDescent="1.25">
       <c r="A1" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1">
+        <v>3</v>
+      </c>
       <c r="D1" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reverted to version 2
</commit_message>
<xml_diff>
--- a/Excel/Excel Test.xlsx
+++ b/Excel/Excel Test.xlsx
@@ -345,22 +345,24 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="90.75" x14ac:dyDescent="1.25">
       <c r="A1" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reverted to version 1
</commit_message>
<xml_diff>
--- a/Excel/Excel Test.xlsx
+++ b/Excel/Excel Test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nigel\Documents\Snirt\Test\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nigel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,18 +25,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="72"/>
-      <color theme="1"/>
-      <name val="Aharoni"/>
     </font>
   </fonts>
   <fills count="2">
@@ -59,9 +54,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,30 +336,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" ht="90.75" x14ac:dyDescent="1.25">
-      <c r="A1" s="1">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>